<commit_message>
revamped teh reservation system
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
+++ b/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Reservation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ECE092-9222-43A5-BF0D-FDC88D9BBB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98A4AAB-CF3A-4ED8-9D43-B609435D2BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Reservation ID</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Table Type</t>
+  </si>
+  <si>
+    <t>Table Count</t>
+  </si>
+  <si>
+    <t>2 seat</t>
+  </si>
+  <si>
+    <t>4 seat</t>
+  </si>
+  <si>
+    <t>10 seat</t>
+  </si>
+  <si>
+    <t>8 seat</t>
   </si>
 </sst>
 </file>
@@ -42,10 +60,16 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy-MM-dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,10 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -390,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,9 +425,11 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.3125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.015625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
+    <col min="5" max="5" width="10.734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +442,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -431,8 +462,14 @@
       <c r="D2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -445,8 +482,14 @@
       <c r="D3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -459,8 +502,14 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -473,36 +522,76 @@
       <c r="D5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45419</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45406</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n">
         <v>4.0</v>
       </c>
-      <c r="C6" t="n" s="2">
-        <v>45419.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C7" t="n" s="3">
-        <v>45406.0</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="C8" t="n" s="2">
+        <v>45410.0</v>
+      </c>
+      <c r="D8" t="n">
         <v>4.0</v>
       </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added jdocs to the reservation controller
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
+++ b/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Reservation ID</t>
   </si>
@@ -95,9 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -414,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -670,6 +671,26 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="n" s="4">
+        <v>45412.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new fields to reservation
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
+++ b/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Reservation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\Reservation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0D3CF2-C27E-4AA5-B2A6-2FA2FCE71223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BFB2DF-77F3-4F15-8BA1-5E653D6443AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Reservation ID</t>
   </si>
@@ -50,15 +50,29 @@
   </si>
   <si>
     <t>8 seat</t>
+  </si>
+  <si>
+    <t>Booking Status</t>
+  </si>
+  <si>
+    <t>Booking Time</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>confirmed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-MM-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -95,12 +109,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,9 +131,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +171,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +277,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,7 +419,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,23 +427,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.05859375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.3125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.015625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +462,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -470,8 +488,14 @@
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -490,8 +514,14 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -510,8 +540,14 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -530,8 +566,14 @@
       <c r="F5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="2">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -550,8 +592,14 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -570,8 +618,14 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="2">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -590,8 +644,14 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -610,8 +670,14 @@
       <c r="F9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -630,65 +696,115 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C11" t="n" s="2">
-        <v>45411.0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10.0</v>
+      <c r="G10" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45411</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B12" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C12" t="n" s="3">
-        <v>45411.0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10.0</v>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45411</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C13" t="n" s="4">
-        <v>45412.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>4.0</v>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45412</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" t="n">
-        <v>1.0</v>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45413</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with the reservation sheet loading and completed code for customer reservation
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
+++ b/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\Reservation\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>Reservation ID</t>
   </si>
@@ -65,14 +65,21 @@
   </si>
   <si>
     <t>confirmed</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>10:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-MM-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,10 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -435,12 +443,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.05859375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.3125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.015625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -622,7 +630,7 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -804,6 +812,32 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="H14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C15" t="n" s="3">
+        <v>45413.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed the waiter page
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
+++ b/Group14-A2/src/main/java/Reservation/ReservationData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\Reservation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\Reservation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BFB2DF-77F3-4F15-8BA1-5E653D6443AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5789AE5-CBBC-45F5-B0E6-D69E93B13C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="852" yWindow="2424" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
   <si>
     <t>Reservation ID</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>confirmed</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
   </si>
   <si>
     <t>10:00</t>
@@ -77,9 +74,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-MM-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -116,11 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,9 +134,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -179,7 +174,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -285,7 +280,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,7 +422,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,20 +433,20 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.05859375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.3125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.015625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.1484375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,10 +495,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -526,10 +521,10 @@
         <v>0.5</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -555,7 +550,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -581,7 +576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -607,7 +602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -630,10 +625,10 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -659,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -685,7 +680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -711,7 +706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -737,7 +732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -763,7 +758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -789,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -815,27 +810,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C15" t="n" s="3">
-        <v>45413.0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>4.0</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45413</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" t="n">
-        <v>2.0</v>
+      <c r="F15">
+        <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>

</xml_diff>